<commit_message>
trivia qs without chemical
</commit_message>
<xml_diff>
--- a/trivia.xlsx
+++ b/trivia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizrts/Documents/llm_eval/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC11B56-EE23-FA45-AA99-547AE07BDB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C679BCF6-6544-444A-BDD5-2176EDA7A977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3940" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="593">
   <si>
     <t>What is the tallest mountain in the world?</t>
   </si>
@@ -517,9 +517,6 @@
     <t>How many chromosomes do humans have?</t>
   </si>
   <si>
-    <t>What is the chemical formula for table salt?</t>
-  </si>
-  <si>
     <t>How many moons does Jupiter have?</t>
   </si>
   <si>
@@ -532,9 +529,6 @@
     <t>Who composed "Symphony No. 5"?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for silver?</t>
-  </si>
-  <si>
     <t>How many bones are in the human spine?</t>
   </si>
   <si>
@@ -547,9 +541,6 @@
     <t>How many states are in the United States?</t>
   </si>
   <si>
-    <t>What is the chemical formula for glucose?</t>
-  </si>
-  <si>
     <t>Who invented the steam engine?</t>
   </si>
   <si>
@@ -559,9 +550,6 @@
     <t>How many chromosomes do chimpanzees have?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for helium?</t>
-  </si>
-  <si>
     <t>Who wrote "War and Peace"?</t>
   </si>
   <si>
@@ -574,27 +562,18 @@
     <t>How many continents were there during the Pangaea period?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for lead?</t>
-  </si>
-  <si>
     <t>What is the smallest ocean on Earth?</t>
   </si>
   <si>
     <t>How many pairs of ribs does a human have?</t>
   </si>
   <si>
-    <t>What is the chemical formula for sulfuric acid?</t>
-  </si>
-  <si>
     <t>What is the most common blood type in humans?</t>
   </si>
   <si>
     <t>How many elements are in the noble gas group?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for potassium?</t>
-  </si>
-  <si>
     <t>Who composed "The Magic Flute"?</t>
   </si>
   <si>
@@ -604,9 +583,6 @@
     <t>How many bones are in the human foot?</t>
   </si>
   <si>
-    <t>What is the chemical formula for methane?</t>
-  </si>
-  <si>
     <t>Who discovered the planet Neptune?</t>
   </si>
   <si>
@@ -622,9 +598,6 @@
     <t>How do you calculate the area of a circle?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for gold?</t>
-  </si>
-  <si>
     <t>What is the fastest land animal?</t>
   </si>
   <si>
@@ -808,9 +781,6 @@
     <t>What is the largest organ in the human body?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for carbon?</t>
-  </si>
-  <si>
     <t>Who painted "The Persistence of Memory"?</t>
   </si>
   <si>
@@ -886,9 +856,6 @@
     <t>How many known dwarf planets are in our solar system?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for uranium?</t>
-  </si>
-  <si>
     <t>Who wrote "Moby-Dick"?</t>
   </si>
   <si>
@@ -898,9 +865,6 @@
     <t>How many taste buds does the average human tongue have?</t>
   </si>
   <si>
-    <t>What is the chemical formula for ethanol?</t>
-  </si>
-  <si>
     <t>Who discovered the law of conservation of mass?</t>
   </si>
   <si>
@@ -919,9 +883,6 @@
     <t>Who discovered the theory of evolution?</t>
   </si>
   <si>
-    <t>What is the chemical formula for ozone?</t>
-  </si>
-  <si>
     <t>Who painted "The Last Supper"?</t>
   </si>
   <si>
@@ -943,9 +904,6 @@
     <t>How many known moons does Saturn have?</t>
   </si>
   <si>
-    <t>What is the chemical formula for caffeine?</t>
-  </si>
-  <si>
     <t>Who discovered the law of gravity?</t>
   </si>
   <si>
@@ -955,9 +913,6 @@
     <t>How many pairs of wings does a bee have?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for platinum?</t>
-  </si>
-  <si>
     <t>Who wrote "The Hunchback of Notre-Dame"?</t>
   </si>
   <si>
@@ -970,9 +925,6 @@
     <t>How many time zones does India have?</t>
   </si>
   <si>
-    <t>What is the chemical formula for nitric acid?</t>
-  </si>
-  <si>
     <t>Who sculpted "David"?</t>
   </si>
   <si>
@@ -991,9 +943,6 @@
     <t>How many known dwarf planets are there in our solar system?</t>
   </si>
   <si>
-    <t>What is the chemical formula for ammonia?</t>
-  </si>
-  <si>
     <t>Who discovered the law of electromagnetism?</t>
   </si>
   <si>
@@ -1003,9 +952,6 @@
     <t>How many pairs of legs does a lobster have?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for iodine?</t>
-  </si>
-  <si>
     <t>Who wrote "The Adventures of Huckleberry Finn"?</t>
   </si>
   <si>
@@ -1027,9 +973,6 @@
     <t>How many time zones does Japan have?</t>
   </si>
   <si>
-    <t>What is the chemical formula for hydrochloric acid?</t>
-  </si>
-  <si>
     <t>Who painted "The Creation of Adam"?</t>
   </si>
   <si>
@@ -1057,9 +1000,6 @@
     <t>How many pairs of wings does a dragonfly have?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for antimony?</t>
-  </si>
-  <si>
     <t>Who wrote "The Tale of Genji"?</t>
   </si>
   <si>
@@ -1105,9 +1045,6 @@
     <t>How many chambers does a nautilus shell have?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for iron?</t>
-  </si>
-  <si>
     <t>Who composed "The Rite of Spring"?</t>
   </si>
   <si>
@@ -1126,9 +1063,6 @@
     <t>Who invented the first successful submarine?</t>
   </si>
   <si>
-    <t>What is the chemical formula for vinegar?</t>
-  </si>
-  <si>
     <t>How many hearts does a squid have?</t>
   </si>
   <si>
@@ -1138,9 +1072,6 @@
     <t>What is the smallest bird in the world?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for nitrogen?</t>
-  </si>
-  <si>
     <t>Who discovered the planet Uranus?</t>
   </si>
   <si>
@@ -1570,9 +1501,6 @@
     <t>What is the main ingredient in kimchi?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for sodium?</t>
-  </si>
-  <si>
     <t>Who wrote "The Count of Monte Cristo"?</t>
   </si>
   <si>
@@ -1594,9 +1522,6 @@
     <t>What is the main ingredient in baba ganoush?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for tungsten?</t>
-  </si>
-  <si>
     <t>How many strings does a harp typically have?</t>
   </si>
   <si>
@@ -1621,9 +1546,6 @@
     <t>What is the main ingredient in tahini?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for mercury?</t>
-  </si>
-  <si>
     <t>Who wrote "The Old Man and the Sea"?</t>
   </si>
   <si>
@@ -1645,9 +1567,6 @@
     <t>What is the main ingredient in sriracha sauce?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for neon?</t>
-  </si>
-  <si>
     <t>How many keys does a standard accordion have?</t>
   </si>
   <si>
@@ -1678,9 +1597,6 @@
     <t>What is the main ingredient in aioli?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for copper?</t>
-  </si>
-  <si>
     <t>Who wrote "One Flew Over the Cuckoo's Nest"?</t>
   </si>
   <si>
@@ -1705,9 +1621,6 @@
     <t>Who discovered the laws of thermodynamics?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for phosphorus?</t>
-  </si>
-  <si>
     <t>How many valves does a trumpet have?</t>
   </si>
   <si>
@@ -1729,9 +1642,6 @@
     <t>What is the main ingredient in gochujang?</t>
   </si>
   <si>
-    <t>What is the chemical symbol for aluminum?</t>
-  </si>
-  <si>
     <t>Who wrote "The Grapes of Wrath"?</t>
   </si>
   <si>
@@ -1886,6 +1796,9 @@
   </si>
   <si>
     <t>What are three famous operas?</t>
+  </si>
+  <si>
+    <t>Who was the first President of the United States?</t>
   </si>
 </sst>
 </file>
@@ -1935,7 +1848,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1948,6 +1861,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2167,15 +2083,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E1050"/>
+  <dimension ref="A1:E1048"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="B187" sqref="B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" customWidth="1"/>
+    <col min="1" max="1" width="30.5" style="5" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
@@ -2191,7 +2107,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2200,7 +2116,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2218,7 +2134,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2344,7 +2260,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -2371,7 +2287,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2425,7 +2341,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -2488,7 +2404,7 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -2497,7 +2413,7 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -2506,7 +2422,7 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -2560,7 +2476,7 @@
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
@@ -2578,7 +2494,7 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
@@ -2596,7 +2512,7 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -2605,7 +2521,7 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
@@ -2632,7 +2548,7 @@
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
@@ -2668,7 +2584,7 @@
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
     </row>
-    <row r="55" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
@@ -2686,7 +2602,7 @@
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
     </row>
-    <row r="57" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
@@ -2722,7 +2638,7 @@
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
     </row>
-    <row r="61" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
@@ -2731,7 +2647,7 @@
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
@@ -2767,7 +2683,7 @@
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
@@ -2857,7 +2773,7 @@
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
     </row>
-    <row r="76" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
@@ -2884,7 +2800,7 @@
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
     </row>
-    <row r="79" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -2920,7 +2836,7 @@
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
     </row>
-    <row r="83" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A83" s="2" t="s">
         <v>82</v>
       </c>
@@ -2956,7 +2872,7 @@
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
     </row>
-    <row r="87" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
@@ -3001,7 +2917,7 @@
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
     </row>
-    <row r="92" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
@@ -3100,7 +3016,7 @@
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
     </row>
-    <row r="103" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
@@ -3145,7 +3061,7 @@
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
     </row>
-    <row r="108" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A108" s="2" t="s">
         <v>107</v>
       </c>
@@ -3172,7 +3088,7 @@
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
     </row>
-    <row r="111" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A111" s="2" t="s">
         <v>110</v>
       </c>
@@ -3226,7 +3142,7 @@
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
     </row>
-    <row r="117" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A117" s="2" t="s">
         <v>116</v>
       </c>
@@ -3307,7 +3223,7 @@
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
     </row>
-    <row r="126" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A126" s="2" t="s">
         <v>125</v>
       </c>
@@ -3334,7 +3250,7 @@
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
     </row>
-    <row r="129" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A129" s="2" t="s">
         <v>128</v>
       </c>
@@ -3343,7 +3259,7 @@
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
     </row>
-    <row r="130" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A130" s="2" t="s">
         <v>129</v>
       </c>
@@ -3370,7 +3286,7 @@
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
     </row>
-    <row r="133" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A133" s="2" t="s">
         <v>132</v>
       </c>
@@ -3388,7 +3304,7 @@
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
     </row>
-    <row r="135" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A135" s="2" t="s">
         <v>134</v>
       </c>
@@ -3424,7 +3340,7 @@
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
     </row>
-    <row r="139" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A139" s="2" t="s">
         <v>138</v>
       </c>
@@ -3442,7 +3358,7 @@
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
     </row>
-    <row r="141" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A141" s="2" t="s">
         <v>140</v>
       </c>
@@ -3451,7 +3367,7 @@
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
     </row>
-    <row r="142" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
         <v>141</v>
       </c>
@@ -3487,7 +3403,7 @@
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
     </row>
-    <row r="146" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
         <v>145</v>
       </c>
@@ -3579,16 +3495,16 @@
     </row>
     <row r="156" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A156" s="2" t="s">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
     </row>
-    <row r="157" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A157" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -3597,7 +3513,7 @@
     </row>
     <row r="158" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A158" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -3606,7 +3522,7 @@
     </row>
     <row r="159" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A159" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -3615,7 +3531,7 @@
     </row>
     <row r="160" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A160" s="2" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -3624,43 +3540,43 @@
     </row>
     <row r="161" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A161" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
     </row>
-    <row r="162" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A162" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
     </row>
-    <row r="163" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A163" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
     </row>
-    <row r="164" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A164" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
     </row>
-    <row r="165" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A165" s="2" t="s">
-        <v>164</v>
+        <v>52</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3669,7 +3585,7 @@
     </row>
     <row r="166" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A166" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3678,16 +3594,16 @@
     </row>
     <row r="167" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A167" s="2" t="s">
-        <v>166</v>
+        <v>592</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
     </row>
-    <row r="168" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A168" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3696,16 +3612,16 @@
     </row>
     <row r="169" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A169" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
     </row>
-    <row r="170" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A170" s="2" t="s">
-        <v>169</v>
+        <v>40</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3714,7 +3630,7 @@
     </row>
     <row r="171" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A171" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3723,7 +3639,7 @@
     </row>
     <row r="172" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A172" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3732,7 +3648,7 @@
     </row>
     <row r="173" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A173" s="2" t="s">
-        <v>172</v>
+        <v>19</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3741,7 +3657,7 @@
     </row>
     <row r="174" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A174" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3750,16 +3666,16 @@
     </row>
     <row r="175" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A175" s="2" t="s">
-        <v>174</v>
+        <v>2</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
     </row>
-    <row r="176" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A176" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3768,25 +3684,25 @@
     </row>
     <row r="177" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A177" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
     </row>
-    <row r="178" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A178" s="2" t="s">
-        <v>177</v>
+        <v>68</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
     </row>
-    <row r="179" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A179" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3795,16 +3711,16 @@
     </row>
     <row r="180" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A180" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
     </row>
-    <row r="181" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A181" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -3813,16 +3729,16 @@
     </row>
     <row r="182" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A182" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
     </row>
-    <row r="183" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A183" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -3831,25 +3747,25 @@
     </row>
     <row r="184" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A184" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
     </row>
-    <row r="185" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A185" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
     </row>
-    <row r="186" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A186" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
@@ -3858,7 +3774,7 @@
     </row>
     <row r="187" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A187" s="2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
@@ -3867,25 +3783,25 @@
     </row>
     <row r="188" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A188" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
     </row>
-    <row r="189" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A189" s="2" t="s">
-        <v>188</v>
+        <v>11</v>
       </c>
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
     </row>
-    <row r="190" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A190" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
@@ -3894,7 +3810,7 @@
     </row>
     <row r="191" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A191" s="2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
@@ -3903,7 +3819,7 @@
     </row>
     <row r="192" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A192" s="2" t="s">
-        <v>191</v>
+        <v>29</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
@@ -3912,7 +3828,7 @@
     </row>
     <row r="193" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A193" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
@@ -3921,16 +3837,16 @@
     </row>
     <row r="194" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A194" s="2" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
     </row>
-    <row r="195" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A195" s="2" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
@@ -3939,7 +3855,7 @@
     </row>
     <row r="196" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A196" s="2" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
@@ -3948,25 +3864,25 @@
     </row>
     <row r="197" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A197" s="2" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
     </row>
-    <row r="198" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A198" s="2" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
       <c r="D198" s="2"/>
       <c r="E198" s="2"/>
     </row>
-    <row r="199" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A199" s="2" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
@@ -3975,7 +3891,7 @@
     </row>
     <row r="200" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A200" s="2" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
@@ -3984,25 +3900,25 @@
     </row>
     <row r="201" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A201" s="2" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B201" s="2"/>
       <c r="C201" s="2"/>
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
     </row>
-    <row r="202" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A202" s="2" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
       <c r="D202" s="2"/>
       <c r="E202" s="2"/>
     </row>
-    <row r="203" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A203" s="2" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
@@ -4011,61 +3927,61 @@
     </row>
     <row r="204" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A204" s="2" t="s">
-        <v>203</v>
+        <v>9</v>
       </c>
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
     </row>
-    <row r="205" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A205" s="2" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
       <c r="D205" s="2"/>
       <c r="E205" s="2"/>
     </row>
-    <row r="206" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A206" s="2" t="s">
-        <v>205</v>
+        <v>42</v>
       </c>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
       <c r="E206" s="2"/>
     </row>
-    <row r="207" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A207" s="2" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
     </row>
-    <row r="208" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A208" s="2" t="s">
-        <v>207</v>
+        <v>4</v>
       </c>
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
     </row>
-    <row r="209" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A209" s="2" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
       <c r="E209" s="2"/>
     </row>
-    <row r="210" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A210" s="2" t="s">
-        <v>209</v>
+        <v>37</v>
       </c>
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
@@ -4074,7 +3990,7 @@
     </row>
     <row r="211" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A211" s="2" t="s">
-        <v>210</v>
+        <v>63</v>
       </c>
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
@@ -4083,16 +3999,16 @@
     </row>
     <row r="212" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A212" s="2" t="s">
-        <v>211</v>
+        <v>8</v>
       </c>
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
       <c r="E212" s="2"/>
     </row>
-    <row r="213" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A213" s="2" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
@@ -4101,7 +4017,7 @@
     </row>
     <row r="214" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A214" s="2" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
@@ -4110,25 +4026,25 @@
     </row>
     <row r="215" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A215" s="2" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
       <c r="E215" s="2"/>
     </row>
-    <row r="216" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A216" s="2" t="s">
-        <v>215</v>
+        <v>27</v>
       </c>
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
       <c r="E216" s="2"/>
     </row>
-    <row r="217" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A217" s="2" t="s">
-        <v>216</v>
+        <v>6</v>
       </c>
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
@@ -4137,34 +4053,34 @@
     </row>
     <row r="218" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A218" s="2" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
       <c r="E218" s="2"/>
     </row>
-    <row r="219" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A219" s="2" t="s">
-        <v>218</v>
+        <v>17</v>
       </c>
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
       <c r="E219" s="2"/>
     </row>
-    <row r="220" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A220" s="2" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
     </row>
-    <row r="221" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A221" s="2" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
@@ -4173,2271 +4089,2433 @@
     </row>
     <row r="222" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A222" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B222" s="2"/>
-      <c r="C222" s="2"/>
-      <c r="D222" s="2"/>
-      <c r="E222" s="2"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="223" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A223" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B223" s="2"/>
-      <c r="C223" s="2"/>
-      <c r="D223" s="2"/>
-      <c r="E223" s="2"/>
+        <v>202</v>
+      </c>
     </row>
     <row r="224" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A224" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A225" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A226" s="2" t="s">
-        <v>225</v>
+        <v>35</v>
       </c>
     </row>
     <row r="227" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A227" s="2" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
     </row>
     <row r="228" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A228" s="2" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
     </row>
     <row r="229" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A229" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="230" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A230" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="231" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A231" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="232" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A232" s="2" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
     </row>
     <row r="233" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A233" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="234" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A234" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="235" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A235" s="2" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
     </row>
     <row r="236" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A236" s="2" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
     </row>
     <row r="237" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A237" s="2" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
     </row>
     <row r="238" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A238" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="239" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A239" s="2" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
     </row>
     <row r="240" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A240" s="2" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
     </row>
     <row r="241" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A241" s="2" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
     </row>
     <row r="242" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A242" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A243" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A244" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
     </row>
     <row r="245" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A245" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A246" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A247" s="2" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
     </row>
     <row r="248" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A248" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="249" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A249" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="250" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A250" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="251" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A251" s="2" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
     </row>
     <row r="252" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A252" s="2" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
     </row>
     <row r="253" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A253" s="2" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
     </row>
     <row r="254" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A254" s="2" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
     </row>
     <row r="255" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A255" s="2" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
     </row>
     <row r="256" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A256" s="2" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
     </row>
     <row r="257" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A257" s="2" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
     </row>
     <row r="258" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A258" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="259" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A259" s="2" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
     </row>
     <row r="260" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A260" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="261" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A261" s="2" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
     </row>
     <row r="262" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A262" s="2" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
     </row>
     <row r="263" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A263" s="2" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="264" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A264" s="2" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="265" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A265" s="2" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
     </row>
     <row r="266" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A266" s="2" t="s">
-        <v>265</v>
+        <v>67</v>
       </c>
     </row>
     <row r="267" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A267" s="2" t="s">
-        <v>266</v>
+        <v>244</v>
       </c>
     </row>
     <row r="268" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A268" s="2" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
     </row>
     <row r="269" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A269" s="2" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
     </row>
     <row r="270" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A270" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="271" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A271" s="2" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
     </row>
     <row r="272" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A272" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="273" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A273" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="274" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A274" s="2" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
     </row>
     <row r="275" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A275" s="2" t="s">
-        <v>274</v>
+        <v>252</v>
       </c>
     </row>
     <row r="276" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A276" s="2" t="s">
-        <v>275</v>
+        <v>253</v>
       </c>
     </row>
     <row r="277" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A277" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="278" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A278" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="279" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A279" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="280" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A280" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="281" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A281" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="282" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A282" s="2" t="s">
-        <v>281</v>
+        <v>46</v>
       </c>
     </row>
     <row r="283" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A283" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="284" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A284" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="285" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A285" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="286" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A286" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="287" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A287" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="288" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A288" s="2" t="s">
-        <v>287</v>
+        <v>10</v>
       </c>
     </row>
     <row r="289" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A289" s="2" t="s">
-        <v>288</v>
+        <v>259</v>
       </c>
     </row>
     <row r="290" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A290" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="291" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A291" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="292" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A292" s="2" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
     </row>
     <row r="293" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A293" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="294" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A294" s="2" t="s">
-        <v>293</v>
+        <v>9</v>
       </c>
     </row>
     <row r="295" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A295" s="2" t="s">
-        <v>294</v>
+        <v>64</v>
       </c>
     </row>
     <row r="296" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A296" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="297" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A297" s="2" t="s">
-        <v>296</v>
+        <v>263</v>
       </c>
     </row>
     <row r="298" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A298" s="2" t="s">
-        <v>297</v>
+        <v>264</v>
       </c>
     </row>
     <row r="299" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A299" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="300" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A300" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="301" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A301" s="2" t="s">
-        <v>300</v>
+        <v>28</v>
       </c>
     </row>
     <row r="302" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A302" s="2" t="s">
-        <v>301</v>
+        <v>267</v>
       </c>
     </row>
     <row r="303" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A303" s="2" t="s">
-        <v>302</v>
+        <v>268</v>
       </c>
     </row>
     <row r="304" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A304" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="305" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A305" s="2" t="s">
-        <v>304</v>
+        <v>270</v>
       </c>
     </row>
     <row r="306" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A306" s="2" t="s">
-        <v>305</v>
+        <v>271</v>
       </c>
     </row>
     <row r="307" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A307" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="308" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A308" s="2" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
     </row>
     <row r="309" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A309" s="2" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
     </row>
     <row r="310" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A310" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="311" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A311" s="2" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
     </row>
     <row r="312" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A312" s="2" t="s">
-        <v>311</v>
+        <v>276</v>
       </c>
     </row>
     <row r="313" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A313" s="2" t="s">
-        <v>312</v>
+        <v>277</v>
       </c>
     </row>
     <row r="314" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A314" s="2" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
     </row>
     <row r="315" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A315" s="2" t="s">
-        <v>314</v>
+        <v>279</v>
       </c>
     </row>
     <row r="316" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A316" s="2" t="s">
-        <v>315</v>
+        <v>280</v>
       </c>
     </row>
     <row r="317" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A317" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="318" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A318" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="319" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A319" s="2" t="s">
-        <v>318</v>
+        <v>283</v>
       </c>
     </row>
     <row r="320" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A320" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="321" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A321" s="2" t="s">
-        <v>320</v>
+        <v>285</v>
       </c>
     </row>
     <row r="322" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A322" s="2" t="s">
-        <v>321</v>
+        <v>286</v>
       </c>
     </row>
     <row r="323" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A323" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="324" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A324" s="2" t="s">
-        <v>323</v>
+        <v>287</v>
       </c>
     </row>
     <row r="325" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A325" s="2" t="s">
-        <v>324</v>
+        <v>288</v>
       </c>
     </row>
     <row r="326" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A326" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="327" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A327" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="328" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A328" s="2" t="s">
-        <v>327</v>
+        <v>291</v>
       </c>
     </row>
     <row r="329" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A329" s="2" t="s">
-        <v>328</v>
+        <v>292</v>
       </c>
     </row>
     <row r="330" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A330" s="2" t="s">
-        <v>329</v>
+        <v>293</v>
       </c>
     </row>
     <row r="331" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A331" s="2" t="s">
-        <v>330</v>
+        <v>294</v>
       </c>
     </row>
     <row r="332" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A332" s="2" t="s">
-        <v>331</v>
+        <v>295</v>
       </c>
     </row>
     <row r="333" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A333" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="334" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A334" s="2" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
     </row>
     <row r="335" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A335" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="336" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A336" s="2" t="s">
-        <v>335</v>
+        <v>298</v>
       </c>
     </row>
     <row r="337" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A337" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="338" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A338" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="339" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A339" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="340" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A340" s="2" t="s">
-        <v>339</v>
+        <v>300</v>
       </c>
     </row>
     <row r="341" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A341" s="2" t="s">
-        <v>340</v>
+        <v>301</v>
       </c>
     </row>
     <row r="342" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A342" s="2" t="s">
-        <v>341</v>
+        <v>302</v>
       </c>
     </row>
     <row r="343" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A343" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="344" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A344" s="2" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
     </row>
     <row r="345" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A345" s="2" t="s">
-        <v>344</v>
+        <v>251</v>
       </c>
     </row>
     <row r="346" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A346" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="347" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A347" s="2" t="s">
-        <v>346</v>
+        <v>306</v>
       </c>
     </row>
     <row r="348" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A348" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="349" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A349" s="2" t="s">
-        <v>348</v>
+        <v>308</v>
       </c>
     </row>
     <row r="350" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A350" s="2" t="s">
-        <v>349</v>
+        <v>309</v>
       </c>
     </row>
     <row r="351" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A351" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="352" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A352" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="353" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A353" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="354" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A354" s="2" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
     </row>
     <row r="355" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A355" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="356" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A356" s="2" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
     </row>
     <row r="357" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A357" s="2" t="s">
-        <v>356</v>
+        <v>316</v>
       </c>
     </row>
     <row r="358" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A358" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="359" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A359" s="2" t="s">
-        <v>358</v>
+        <v>318</v>
       </c>
     </row>
     <row r="360" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A360" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="361" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A361" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="362" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A362" s="2" t="s">
-        <v>361</v>
+        <v>321</v>
       </c>
     </row>
     <row r="363" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A363" s="2" t="s">
-        <v>362</v>
+        <v>322</v>
       </c>
     </row>
     <row r="364" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A364" s="2" t="s">
-        <v>363</v>
+        <v>323</v>
       </c>
     </row>
     <row r="365" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A365" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="366" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A366" s="2" t="s">
-        <v>365</v>
+        <v>276</v>
       </c>
     </row>
     <row r="367" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A367" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="368" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A368" s="2" t="s">
-        <v>367</v>
+        <v>326</v>
       </c>
     </row>
     <row r="369" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A369" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="370" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A370" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="371" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A371" s="2" t="s">
-        <v>370</v>
+        <v>329</v>
       </c>
     </row>
     <row r="372" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A372" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="373" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A373" s="2" t="s">
-        <v>372</v>
+        <v>331</v>
       </c>
     </row>
     <row r="374" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A374" s="2" t="s">
-        <v>373</v>
+        <v>332</v>
       </c>
     </row>
     <row r="375" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A375" s="2" t="s">
-        <v>374</v>
+        <v>333</v>
       </c>
     </row>
     <row r="376" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A376" s="2" t="s">
-        <v>375</v>
+        <v>334</v>
       </c>
     </row>
     <row r="377" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A377" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="378" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A378" s="2" t="s">
-        <v>377</v>
+        <v>336</v>
       </c>
     </row>
     <row r="379" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A379" s="2" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="380" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A380" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="381" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A381" s="2" t="s">
-        <v>380</v>
+        <v>338</v>
       </c>
     </row>
     <row r="382" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A382" s="2" t="s">
-        <v>381</v>
+        <v>339</v>
       </c>
     </row>
     <row r="383" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A383" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="384" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A384" s="2" t="s">
-        <v>383</v>
+        <v>341</v>
       </c>
     </row>
     <row r="385" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A385" s="2" t="s">
-        <v>384</v>
+        <v>342</v>
       </c>
     </row>
     <row r="386" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A386" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="387" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A387" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="388" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A388" s="2" t="s">
-        <v>387</v>
+        <v>345</v>
       </c>
     </row>
     <row r="389" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A389" s="2" t="s">
-        <v>388</v>
+        <v>346</v>
       </c>
     </row>
     <row r="390" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A390" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="391" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A391" s="2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="392" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A392" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="393" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A393" s="2" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="394" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A394" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="395" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A395" s="2" t="s">
-        <v>394</v>
+        <v>352</v>
       </c>
     </row>
     <row r="396" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A396" s="2" t="s">
-        <v>395</v>
+        <v>353</v>
       </c>
     </row>
     <row r="397" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A397" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="398" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A398" s="2" t="s">
-        <v>397</v>
+        <v>355</v>
       </c>
     </row>
     <row r="399" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A399" s="2" t="s">
-        <v>398</v>
+        <v>356</v>
       </c>
     </row>
     <row r="400" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A400" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="401" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A401" s="2" t="s">
-        <v>400</v>
+        <v>358</v>
       </c>
     </row>
     <row r="402" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A402" s="2" t="s">
-        <v>401</v>
+        <v>359</v>
       </c>
     </row>
     <row r="403" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A403" s="2" t="s">
-        <v>402</v>
+        <v>360</v>
       </c>
     </row>
     <row r="404" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A404" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
     </row>
     <row r="405" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A405" s="2" t="s">
-        <v>404</v>
+        <v>47</v>
       </c>
     </row>
     <row r="406" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A406" s="2" t="s">
-        <v>405</v>
+        <v>362</v>
       </c>
     </row>
     <row r="407" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A407" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="408" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A408" s="2" t="s">
-        <v>407</v>
+        <v>364</v>
       </c>
     </row>
     <row r="409" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A409" s="2" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="410" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A410" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="411" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A411" s="2" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="412" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A412" s="2" t="s">
-        <v>411</v>
+        <v>367</v>
       </c>
     </row>
     <row r="413" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A413" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="414" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A414" s="2" t="s">
-        <v>413</v>
+        <v>368</v>
       </c>
     </row>
     <row r="415" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A415" s="2" t="s">
-        <v>414</v>
+        <v>153</v>
       </c>
     </row>
     <row r="416" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A416" s="2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="417" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A417" s="2" t="s">
-        <v>416</v>
+        <v>194</v>
       </c>
     </row>
     <row r="418" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A418" s="2" t="s">
-        <v>417</v>
+        <v>161</v>
       </c>
     </row>
     <row r="419" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A419" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="420" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A420" s="2" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="421" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A421" s="2" t="s">
-        <v>420</v>
+        <v>372</v>
       </c>
     </row>
     <row r="422" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A422" s="2" t="s">
-        <v>421</v>
+        <v>373</v>
       </c>
     </row>
     <row r="423" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A423" s="2" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="424" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A424" s="2" t="s">
-        <v>423</v>
+        <v>375</v>
       </c>
     </row>
     <row r="425" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A425" s="2" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="426" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A426" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="427" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A427" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="428" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A428" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="429" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A429" s="2" t="s">
-        <v>428</v>
+        <v>9</v>
       </c>
     </row>
     <row r="430" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A430" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="431" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A431" s="2" t="s">
-        <v>430</v>
+        <v>381</v>
       </c>
     </row>
     <row r="432" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A432" s="2" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="433" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A433" s="2" t="s">
-        <v>432</v>
+        <v>383</v>
       </c>
     </row>
     <row r="434" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A434" s="2" t="s">
-        <v>433</v>
+        <v>384</v>
       </c>
     </row>
     <row r="435" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A435" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="436" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A436" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="437" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A437" s="2" t="s">
-        <v>436</v>
+        <v>387</v>
       </c>
     </row>
     <row r="438" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A438" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="439" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A439" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="440" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A440" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="441" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A441" s="2" t="s">
-        <v>440</v>
+        <v>391</v>
       </c>
     </row>
     <row r="442" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A442" s="2" t="s">
-        <v>441</v>
+        <v>392</v>
       </c>
     </row>
     <row r="443" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A443" s="2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="444" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A444" s="2" t="s">
-        <v>443</v>
+        <v>394</v>
       </c>
     </row>
     <row r="445" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A445" s="2" t="s">
-        <v>444</v>
+        <v>395</v>
       </c>
     </row>
     <row r="446" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A446" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="447" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A447" s="2" t="s">
-        <v>446</v>
+        <v>397</v>
       </c>
     </row>
     <row r="448" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A448" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="449" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A449" s="2" t="s">
-        <v>448</v>
+        <v>399</v>
       </c>
     </row>
     <row r="450" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A450" s="2" t="s">
-        <v>449</v>
+        <v>400</v>
       </c>
     </row>
     <row r="451" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A451" s="2" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="452" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A452" s="2" t="s">
-        <v>451</v>
+        <v>402</v>
       </c>
     </row>
     <row r="453" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A453" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="454" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A454" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="455" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A455" s="2" t="s">
-        <v>454</v>
+        <v>405</v>
       </c>
     </row>
     <row r="456" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A456" s="2" t="s">
-        <v>455</v>
+        <v>406</v>
       </c>
     </row>
     <row r="457" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A457" s="2" t="s">
-        <v>456</v>
+        <v>407</v>
       </c>
     </row>
     <row r="458" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A458" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="459" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A459" s="2" t="s">
-        <v>458</v>
+        <v>409</v>
       </c>
     </row>
     <row r="460" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A460" s="2" t="s">
-        <v>459</v>
+        <v>360</v>
       </c>
     </row>
     <row r="461" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A461" s="2" t="s">
-        <v>460</v>
+        <v>410</v>
       </c>
     </row>
     <row r="462" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A462" s="2" t="s">
-        <v>461</v>
+        <v>411</v>
       </c>
     </row>
     <row r="463" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A463" s="2" t="s">
-        <v>462</v>
+        <v>412</v>
       </c>
     </row>
     <row r="464" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A464" s="2" t="s">
-        <v>463</v>
+        <v>413</v>
       </c>
     </row>
     <row r="465" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A465" s="2" t="s">
-        <v>464</v>
+        <v>414</v>
       </c>
     </row>
     <row r="466" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A466" s="2" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="467" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A467" s="2" t="s">
-        <v>466</v>
+        <v>416</v>
       </c>
     </row>
     <row r="468" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A468" s="2" t="s">
-        <v>467</v>
+        <v>417</v>
       </c>
     </row>
     <row r="469" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A469" s="2" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="470" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A470" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="471" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A471" s="2" t="s">
-        <v>470</v>
+        <v>420</v>
       </c>
     </row>
     <row r="472" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A472" s="2" t="s">
-        <v>471</v>
+        <v>421</v>
       </c>
     </row>
     <row r="473" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A473" s="2" t="s">
-        <v>472</v>
+        <v>422</v>
       </c>
     </row>
     <row r="474" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A474" s="2" t="s">
-        <v>473</v>
+        <v>423</v>
       </c>
     </row>
     <row r="475" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A475" s="2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="476" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A476" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="477" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A477" s="2" t="s">
-        <v>476</v>
+        <v>426</v>
       </c>
     </row>
     <row r="478" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A478" s="2" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="479" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A479" s="2" t="s">
-        <v>478</v>
+        <v>428</v>
       </c>
     </row>
     <row r="480" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A480" s="2" t="s">
-        <v>479</v>
+        <v>353</v>
       </c>
     </row>
     <row r="481" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A481" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="482" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A482" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="483" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A483" s="2" t="s">
-        <v>482</v>
+        <v>431</v>
       </c>
     </row>
     <row r="484" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A484" s="2" t="s">
-        <v>483</v>
+        <v>432</v>
       </c>
     </row>
     <row r="485" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A485" s="2" t="s">
-        <v>484</v>
+        <v>433</v>
       </c>
     </row>
     <row r="486" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A486" s="2" t="s">
-        <v>485</v>
+        <v>434</v>
       </c>
     </row>
     <row r="487" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A487" s="2" t="s">
-        <v>486</v>
+        <v>435</v>
       </c>
     </row>
     <row r="488" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A488" s="2" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="489" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A489" s="2" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="490" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A490" s="2" t="s">
-        <v>489</v>
+        <v>438</v>
       </c>
     </row>
     <row r="491" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A491" s="2" t="s">
-        <v>490</v>
+        <v>439</v>
       </c>
     </row>
     <row r="492" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A492" s="2" t="s">
-        <v>491</v>
+        <v>203</v>
       </c>
     </row>
     <row r="493" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A493" s="2" t="s">
-        <v>492</v>
+        <v>440</v>
       </c>
     </row>
     <row r="494" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A494" s="2" t="s">
-        <v>493</v>
+        <v>441</v>
       </c>
     </row>
     <row r="495" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A495" s="2" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="496" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A496" s="2" t="s">
-        <v>495</v>
+        <v>443</v>
       </c>
     </row>
     <row r="497" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A497" s="2" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="498" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A498" s="2" t="s">
-        <v>497</v>
+        <v>445</v>
       </c>
     </row>
     <row r="499" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A499" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="500" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A500" s="2" t="s">
-        <v>499</v>
+        <v>447</v>
       </c>
     </row>
     <row r="501" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A501" s="2" t="s">
-        <v>500</v>
+        <v>448</v>
       </c>
     </row>
     <row r="502" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A502" s="2" t="s">
-        <v>501</v>
+        <v>449</v>
       </c>
     </row>
     <row r="503" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A503" s="2" t="s">
-        <v>502</v>
+        <v>450</v>
       </c>
     </row>
     <row r="504" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A504" s="2" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="505" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A505" s="2" t="s">
-        <v>504</v>
+        <v>452</v>
       </c>
     </row>
     <row r="506" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A506" s="2" t="s">
-        <v>505</v>
+        <v>63</v>
       </c>
     </row>
     <row r="507" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A507" s="2" t="s">
-        <v>506</v>
+        <v>372</v>
       </c>
     </row>
     <row r="508" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A508" s="2" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="509" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A509" s="2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="510" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A510" s="2" t="s">
-        <v>509</v>
+        <v>455</v>
       </c>
     </row>
     <row r="511" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A511" s="2" t="s">
-        <v>510</v>
+        <v>456</v>
       </c>
     </row>
     <row r="512" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A512" s="2" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="513" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A513" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="514" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A514" s="2" t="s">
-        <v>513</v>
+        <v>459</v>
       </c>
     </row>
     <row r="515" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A515" s="2" t="s">
-        <v>514</v>
+        <v>460</v>
       </c>
     </row>
     <row r="516" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A516" s="2" t="s">
-        <v>515</v>
+        <v>461</v>
       </c>
     </row>
     <row r="517" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A517" s="2" t="s">
-        <v>516</v>
+        <v>462</v>
       </c>
     </row>
     <row r="518" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A518" s="2" t="s">
-        <v>517</v>
+        <v>463</v>
       </c>
     </row>
     <row r="519" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A519" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="520" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A520" s="2" t="s">
-        <v>519</v>
+        <v>214</v>
       </c>
     </row>
     <row r="521" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A521" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="522" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A522" s="2" t="s">
-        <v>521</v>
+        <v>465</v>
       </c>
     </row>
     <row r="523" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A523" s="2" t="s">
-        <v>522</v>
+        <v>466</v>
       </c>
     </row>
     <row r="524" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A524" s="2" t="s">
-        <v>523</v>
+        <v>467</v>
       </c>
     </row>
     <row r="525" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A525" s="2" t="s">
-        <v>524</v>
+        <v>468</v>
       </c>
     </row>
     <row r="526" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A526" s="2" t="s">
-        <v>525</v>
+        <v>469</v>
       </c>
     </row>
     <row r="527" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A527" s="2" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="528" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A528" s="2" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="529" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A529" s="2" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="530" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A530" s="2" t="s">
-        <v>529</v>
+        <v>201</v>
       </c>
     </row>
     <row r="531" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A531" s="2" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="532" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A532" s="2" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="533" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A533" s="2" t="s">
-        <v>532</v>
+        <v>475</v>
       </c>
     </row>
     <row r="534" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A534" s="2" t="s">
-        <v>533</v>
+        <v>215</v>
       </c>
     </row>
     <row r="535" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A535" s="2" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="536" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A536" s="2" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="537" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A537" s="2" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="538" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A538" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="539" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A539" s="2" t="s">
-        <v>538</v>
+        <v>478</v>
       </c>
     </row>
     <row r="540" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A540" s="2" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="541" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A541" s="2" t="s">
-        <v>540</v>
+        <v>480</v>
       </c>
     </row>
     <row r="542" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A542" s="2" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="543" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A543" s="2" t="s">
-        <v>542</v>
+        <v>482</v>
       </c>
     </row>
     <row r="544" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A544" s="2" t="s">
-        <v>543</v>
+        <v>193</v>
       </c>
     </row>
     <row r="545" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A545" s="2" t="s">
-        <v>544</v>
+        <v>158</v>
       </c>
     </row>
     <row r="546" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A546" s="2" t="s">
-        <v>545</v>
+        <v>483</v>
       </c>
     </row>
     <row r="547" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A547" s="2" t="s">
-        <v>546</v>
+        <v>202</v>
       </c>
     </row>
     <row r="548" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A548" s="2" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="549" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="549" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A549" s="2" t="s">
-        <v>548</v>
+        <v>485</v>
       </c>
     </row>
     <row r="550" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A550" s="2" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="551" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A551" s="2" t="s">
-        <v>550</v>
+        <v>487</v>
       </c>
     </row>
     <row r="552" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A552" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="553" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="553" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A553" s="2" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="554" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="554" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A554" s="2" t="s">
-        <v>553</v>
+        <v>490</v>
       </c>
     </row>
     <row r="555" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A555" s="2" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="556" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="556" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A556" s="2" t="s">
-        <v>555</v>
+        <v>492</v>
       </c>
     </row>
     <row r="557" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A557" s="2" t="s">
-        <v>556</v>
+        <v>493</v>
       </c>
     </row>
     <row r="558" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A558" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="559" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="559" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A559" s="2" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="560" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="560" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A560" s="2" t="s">
-        <v>559</v>
+        <v>496</v>
       </c>
     </row>
     <row r="561" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A561" s="2" t="s">
-        <v>560</v>
+        <v>497</v>
       </c>
     </row>
     <row r="562" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A562" s="2" t="s">
-        <v>561</v>
+        <v>498</v>
       </c>
     </row>
     <row r="563" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A563" s="2" t="s">
-        <v>562</v>
+        <v>499</v>
       </c>
     </row>
     <row r="564" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A564" s="2" t="s">
-        <v>563</v>
+        <v>363</v>
       </c>
     </row>
     <row r="565" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A565" s="2" t="s">
-        <v>564</v>
+        <v>500</v>
       </c>
     </row>
     <row r="566" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A566" s="2" t="s">
-        <v>565</v>
+        <v>477</v>
       </c>
     </row>
     <row r="567" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A567" s="2" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="568" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="568" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A568" s="2" t="s">
-        <v>567</v>
+        <v>502</v>
       </c>
     </row>
     <row r="569" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A569" s="2" t="s">
-        <v>568</v>
+        <v>503</v>
       </c>
     </row>
     <row r="570" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A570" s="2" t="s">
-        <v>569</v>
+        <v>504</v>
       </c>
     </row>
     <row r="571" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A571" s="2" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="572" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="572" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A572" s="2" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="573" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="573" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A573" s="2" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="574" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="574" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A574" s="2" t="s">
-        <v>573</v>
+        <v>507</v>
       </c>
     </row>
     <row r="575" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A575" s="2" t="s">
-        <v>574</v>
+        <v>508</v>
       </c>
     </row>
     <row r="576" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A576" s="2" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="577" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="577" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A577" s="2" t="s">
-        <v>576</v>
+        <v>510</v>
       </c>
     </row>
     <row r="578" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A578" s="2" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="579" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="579" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A579" s="2" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="580" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="580" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A580" s="2" t="s">
-        <v>579</v>
+        <v>513</v>
       </c>
     </row>
     <row r="581" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A581" s="2" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="582" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="582" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A582" s="2" t="s">
-        <v>581</v>
+        <v>357</v>
       </c>
     </row>
     <row r="583" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A583" s="2" t="s">
-        <v>582</v>
+        <v>515</v>
       </c>
     </row>
     <row r="584" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A584" s="2" t="s">
-        <v>583</v>
+        <v>516</v>
       </c>
     </row>
     <row r="585" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A585" s="2" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="586" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="586" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A586" s="2" t="s">
-        <v>585</v>
+        <v>518</v>
       </c>
     </row>
     <row r="587" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A587" s="2" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="588" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="588" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A588" s="2" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="589" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="589" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A589" s="2" t="s">
-        <v>588</v>
+        <v>521</v>
       </c>
     </row>
     <row r="590" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A590" s="2" t="s">
-        <v>589</v>
+        <v>522</v>
       </c>
     </row>
     <row r="591" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A591" s="2" t="s">
-        <v>590</v>
+        <v>523</v>
       </c>
     </row>
     <row r="592" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A592" s="2" t="s">
-        <v>591</v>
+        <v>524</v>
       </c>
     </row>
     <row r="593" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A593" s="2" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="594" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A594" s="2" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="595" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A595" s="2" t="s">
-        <v>594</v>
+        <v>527</v>
       </c>
     </row>
     <row r="596" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A596" s="2" t="s">
-        <v>595</v>
+        <v>528</v>
       </c>
     </row>
     <row r="597" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A597" s="2" t="s">
-        <v>596</v>
+        <v>529</v>
       </c>
     </row>
     <row r="598" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A598" s="2" t="s">
-        <v>597</v>
+        <v>530</v>
       </c>
     </row>
     <row r="599" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A599" s="2" t="s">
-        <v>598</v>
+        <v>531</v>
       </c>
     </row>
     <row r="600" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A600" s="2" t="s">
-        <v>599</v>
+        <v>532</v>
       </c>
     </row>
     <row r="601" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A601" s="2" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="602" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="602" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A602" s="2" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="603" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="603" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A603" s="2" t="s">
-        <v>602</v>
+        <v>535</v>
       </c>
     </row>
     <row r="604" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A604" s="2" t="s">
-        <v>603</v>
+        <v>259</v>
       </c>
     </row>
     <row r="605" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A605" s="2" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="606" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="606" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A606" s="2" t="s">
-        <v>605</v>
+        <v>505</v>
       </c>
     </row>
     <row r="607" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A607" s="2" t="s">
-        <v>606</v>
+        <v>537</v>
       </c>
     </row>
     <row r="608" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A608" s="2" t="s">
-        <v>607</v>
+        <v>538</v>
       </c>
     </row>
     <row r="609" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A609" s="2" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="610" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="610" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A610" s="2" t="s">
-        <v>609</v>
+        <v>540</v>
       </c>
     </row>
     <row r="611" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A611" s="2" t="s">
-        <v>610</v>
+        <v>541</v>
       </c>
     </row>
     <row r="612" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A612" s="2" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="613" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="613" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A613" s="2" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="614" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="614" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A614" s="2" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="615" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="615" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A615" s="2" t="s">
-        <v>614</v>
+        <v>11</v>
       </c>
     </row>
     <row r="616" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A616" s="2" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="617" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="617" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A617" s="2" t="s">
-        <v>616</v>
+        <v>545</v>
       </c>
     </row>
     <row r="618" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A618" s="2" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="619" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="619" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A619" s="2" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="620" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="620" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A620" s="2" t="s">
-        <v>619</v>
+        <v>548</v>
       </c>
     </row>
     <row r="621" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A621" s="2" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="622" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="622" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A622" s="2" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="623" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A623" s="2"/>
-    </row>
-    <row r="624" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A624" s="2"/>
-    </row>
-    <row r="625" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A625" s="2"/>
-    </row>
-    <row r="626" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A626" s="2"/>
-    </row>
-    <row r="627" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A627" s="2"/>
-    </row>
-    <row r="628" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A628" s="2"/>
-    </row>
-    <row r="629" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A629" s="2"/>
-    </row>
-    <row r="630" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A630" s="2"/>
-    </row>
-    <row r="631" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A631" s="2"/>
-    </row>
-    <row r="632" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A632" s="2"/>
-    </row>
-    <row r="633" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A633" s="2"/>
-    </row>
-    <row r="634" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A634" s="2"/>
-    </row>
-    <row r="635" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A635" s="2"/>
-    </row>
-    <row r="636" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A636" s="2"/>
-    </row>
-    <row r="637" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A637" s="2"/>
-    </row>
-    <row r="638" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A638" s="2"/>
-    </row>
-    <row r="639" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A639" s="2"/>
-    </row>
-    <row r="640" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A640" s="2"/>
-    </row>
-    <row r="641" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A641" s="2"/>
-    </row>
-    <row r="642" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A642" s="2"/>
-    </row>
-    <row r="643" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A643" s="2"/>
-    </row>
-    <row r="644" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A644" s="2"/>
-    </row>
-    <row r="645" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A645" s="2"/>
-    </row>
-    <row r="646" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A646" s="2"/>
-    </row>
-    <row r="647" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A647" s="2"/>
-    </row>
-    <row r="648" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A648" s="2"/>
-    </row>
-    <row r="649" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A649" s="2"/>
-    </row>
-    <row r="650" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A650" s="2"/>
-    </row>
-    <row r="651" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A651" s="2"/>
-    </row>
-    <row r="652" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A652" s="2"/>
-    </row>
-    <row r="653" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A653" s="2"/>
-    </row>
-    <row r="654" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A654" s="2"/>
-    </row>
-    <row r="655" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A655" s="2"/>
-    </row>
-    <row r="656" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A656" s="2"/>
-    </row>
-    <row r="657" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A657" s="2"/>
-    </row>
-    <row r="658" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A658" s="2"/>
-    </row>
-    <row r="659" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A659" s="2"/>
-    </row>
-    <row r="660" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A660" s="2"/>
-    </row>
-    <row r="661" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A661" s="2"/>
-    </row>
-    <row r="662" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A662" s="2"/>
-    </row>
-    <row r="663" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A663" s="2"/>
-    </row>
-    <row r="664" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A664" s="2"/>
-    </row>
-    <row r="665" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A665" s="2"/>
-    </row>
-    <row r="666" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A666" s="2"/>
-    </row>
-    <row r="667" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A667" s="2"/>
-    </row>
-    <row r="668" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A668" s="2"/>
-    </row>
-    <row r="669" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A669" s="2"/>
-    </row>
-    <row r="670" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A670" s="2"/>
-    </row>
-    <row r="671" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A671" s="2"/>
-    </row>
-    <row r="672" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A672" s="2"/>
-    </row>
-    <row r="673" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A673" s="2"/>
-    </row>
-    <row r="674" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A674" s="2"/>
-    </row>
-    <row r="675" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A675" s="2"/>
-    </row>
-    <row r="676" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A676" s="2"/>
-    </row>
-    <row r="677" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A677" s="2"/>
-    </row>
-    <row r="678" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A678" s="2"/>
-    </row>
-    <row r="679" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A679" s="2"/>
-    </row>
-    <row r="680" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A680" s="2"/>
-    </row>
-    <row r="681" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A681" s="2"/>
-    </row>
-    <row r="682" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A682" s="2"/>
-    </row>
-    <row r="683" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A683" s="2"/>
-    </row>
-    <row r="684" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A684" s="2"/>
-    </row>
-    <row r="685" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A685" s="2"/>
-    </row>
-    <row r="686" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A686" s="2"/>
-    </row>
-    <row r="687" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A687" s="2"/>
-    </row>
-    <row r="688" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A688" s="2"/>
-    </row>
-    <row r="689" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A689" s="2"/>
-    </row>
-    <row r="690" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A690" s="2"/>
-    </row>
-    <row r="691" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A691" s="2"/>
-    </row>
-    <row r="692" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A692" s="2"/>
-    </row>
-    <row r="693" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A693" s="2"/>
-    </row>
-    <row r="694" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A694" s="2"/>
-    </row>
-    <row r="695" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A695" s="2"/>
-    </row>
-    <row r="696" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A696" s="2"/>
-    </row>
-    <row r="697" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A697" s="2"/>
-    </row>
-    <row r="698" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A698" s="2"/>
-    </row>
-    <row r="699" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A699" s="2"/>
-    </row>
-    <row r="700" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A700" s="2"/>
-    </row>
-    <row r="701" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A701" s="2"/>
-    </row>
-    <row r="702" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A702" s="2"/>
-    </row>
-    <row r="703" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A703" s="2"/>
-    </row>
-    <row r="704" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A704" s="2"/>
-    </row>
-    <row r="705" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A705" s="2"/>
-    </row>
-    <row r="706" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A706" s="2"/>
-    </row>
-    <row r="707" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A707" s="2"/>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="623" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A623" s="2" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A624" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="625" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A625" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="626" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A626" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="627" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A627" s="2" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="628" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A628" s="2" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="629" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A629" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="630" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A630" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="631" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A631" s="2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="632" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A632" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="633" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A633" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="634" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A634" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="635" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A635" s="2" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="636" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A636" s="2" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="637" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A637" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="638" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A638" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="639" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A639" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="640" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A640" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="641" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A641" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="642" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A642" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="643" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A643" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="644" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A644" s="2" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="645" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A645" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="646" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A646" s="2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="647" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A647" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="648" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A648" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="649" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A649" s="2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="650" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A650" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="651" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A651" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="652" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A652" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="653" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A653" s="2" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="654" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A654" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="655" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A655" s="2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="656" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A656" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="657" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A657" s="2" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="658" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A658" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="659" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A659" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="660" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A660" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="661" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A661" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="662" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A662" s="2" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="663" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A663" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="664" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A664" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="665" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A665" s="2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="666" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A666" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="667" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A667" s="2" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="668" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A668" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="669" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A669" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="670" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A670" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="671" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A671" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="672" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A672" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="673" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A673" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="674" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A674" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="675" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A675" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="676" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A676" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="677" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A677" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="678" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A678" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="679" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A679" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="680" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A680" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="681" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A681" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="682" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A682" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="683" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A683" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="684" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A684" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="685" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A685" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="686" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A686" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="687" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A687" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="688" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A688" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="689" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A689" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="690" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A690" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="691" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A691" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="692" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A692" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="693" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A693" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="694" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A694" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="695" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A695" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="696" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A696" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="697" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A697" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="698" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A698" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="699" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A699" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="700" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A700" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="701" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A701" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="702" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A702" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="703" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A703" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="704" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A704" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="705" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A705" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="706" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A706" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="707" spans="1:1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A707" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="708" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A708" s="2"/>
@@ -7461,12 +7539,6 @@
     </row>
     <row r="1048" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1048" s="2"/>
-    </row>
-    <row r="1049" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1049" s="2"/>
-    </row>
-    <row r="1050" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1050" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>